<commit_message>
f/abaird-sleep: updates to metabolic relationships and updates to some validation data
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/NervousValidation.xlsx
+++ b/share/doc/validation/Scenarios/NervousValidation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGearsResearch\sleep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGears\biogears\core\share\doc\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -227,34 +227,34 @@
     <t xml:space="preserve">sleep deprivation study taken from spiegle, given carb rich meal (62%) every 5h </t>
   </si>
   <si>
-    <t>40% lower (1.42%/min compared to 2.4%/min @cite gutierrez2004clinical</t>
-  </si>
-  <si>
     <t>Glucose clearance (%/min)</t>
   </si>
   <si>
     <t>Glucose effectiveness (%/min) clearance without insulin</t>
   </si>
   <si>
-    <t>Decrease 30% @cite Hosomi1979effect @cite Ottesen2004applied</t>
-  </si>
-  <si>
     <t xml:space="preserve">Insulin response (pmol/min) </t>
   </si>
   <si>
-    <t>Decrease from 432 to 304 pmol/min @cite Hosomi1979effect @cite Ottesen2004applied</t>
-  </si>
-  <si>
     <t>Stanford sleepyness score (unitless)</t>
   </si>
   <si>
-    <t>Increase from 2.1 to 4.4 @cite Hosomi1979effect @cite Ottesen2004applied</t>
-  </si>
-  <si>
     <t>Cerebral glucose uptake (% from baseline)</t>
   </si>
   <si>
-    <t>Decrease of 7% @cite Hosomi1979effect @cite Ottesen2004applied</t>
+    <t>40% lower (1.42%/min compared to 2.4%/min @cite spiegel1999impact</t>
+  </si>
+  <si>
+    <t>Decrease 30% @cite spiegel1999impact</t>
+  </si>
+  <si>
+    <t>Decrease from 432 to 304 pmol/min @cite spiegel1999impact</t>
+  </si>
+  <si>
+    <t>Increase from 2.1 to 4.4  @cite spiegel1999impact</t>
+  </si>
+  <si>
+    <t>Decrease of 7% @cite spiegel1999impact</t>
   </si>
 </sst>
 </file>
@@ -1773,8 +1773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,31 +1835,31 @@
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>9</v>
@@ -1941,25 +1941,25 @@
         <v>19</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="L4" s="41" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>55</v>
@@ -2458,18 +2458,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2587,6 +2587,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6320210A-C44C-4B82-8349-5A58CB3B5A77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2597,14 +2605,6 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
f/abaird-sleep: Updates to xmls and a few minor changes
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/NervousValidation.xlsx
+++ b/share/doc/validation/Scenarios/NervousValidation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="80">
   <si>
     <t xml:space="preserve">Scenario </t>
   </si>
@@ -224,9 +224,6 @@
     <t>Sampled Scenario Time (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">sleep deprivation study taken from spiegle, given carb rich meal (62%) every 5h </t>
-  </si>
-  <si>
     <t>Glucose clearance (%/min)</t>
   </si>
   <si>
@@ -255,6 +252,21 @@
   </si>
   <si>
     <t>Decrease of 7% @cite spiegel1999impact</t>
+  </si>
+  <si>
+    <t>Reaction Time (ms)</t>
+  </si>
+  <si>
+    <t>Attention Lapses (% from baseline)</t>
+  </si>
+  <si>
+    <t>Increase ~1000% @cite mchill2018chronic</t>
+  </si>
+  <si>
+    <t>Increase of 100% @cite mchill2018chronic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sleep deprivation study taken from spiegle and McHill, given carb rich meal (62%) every 5h </t>
   </si>
 </sst>
 </file>
@@ -427,7 +439,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -611,6 +623,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -803,7 +821,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,6 +948,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1771,10 +1792,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,9 +1814,11 @@
     <col min="12" max="12" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="33.140625" customWidth="1"/>
     <col min="16" max="16" width="26.7109375" customWidth="1"/>
+    <col min="18" max="18" width="29.85546875" customWidth="1"/>
+    <col min="20" max="20" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4" t="s">
         <v>62</v>
@@ -1812,7 +1835,7 @@
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
     </row>
-    <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -1835,37 +1858,49 @@
         <v>9</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="Q2" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
@@ -1917,8 +1952,20 @@
       <c r="Q3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="R3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1929,7 +1976,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
@@ -1941,33 +1988,45 @@
         <v>19</v>
       </c>
       <c r="H4" s="43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="6" t="s">
-        <v>72</v>
+      <c r="J4" s="44" t="s">
+        <v>71</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="L4" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="N4" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>55</v>
       </c>
       <c r="P4" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="U4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2458,21 +2517,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D00DDCF912707249810263345C6FBCAE" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="05fc12c866532ec63d2052ef81b63530">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="711b5f35d88f7f6ebfe284b0f73f4393">
     <xsd:element name="properties">
@@ -2586,10 +2630,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000C402D-5B8F-44E9-B6EC-AD906C5241AB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2610,17 +2677,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{000C402D-5B8F-44E9-B6EC-AD906C5241AB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1B20E2-65A5-4DC5-B5E1-EAEF16402220}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>